<commit_message>
Added review comment in the post negative scenario
</commit_message>
<xml_diff>
--- a/tests/artifact/script/CustomerandSupplier.xlsx
+++ b/tests/artifact/script/CustomerandSupplier.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500" firstSheet="5" activeTab="8"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1999" uniqueCount="913">
   <si>
     <t>target</t>
   </si>
@@ -2766,6 +2766,9 @@
     <t>Create a new customer / supplier with invalid data: POST- /customer</t>
   </si>
   <si>
+    <t>You can add try creating an existing customer</t>
+  </si>
+  <si>
     <t>iterating the steps using repeatuntil</t>
   </si>
   <si>
@@ -2960,7 +2963,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3028,6 +3031,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.0499893185216834"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
@@ -3549,14 +3559,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3565,119 +3572,122 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3865,10 +3875,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3897,7 +3911,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4265,7 +4279,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="18" width="8.33333333333333" customWidth="1" collapsed="1"/>
   </cols>
@@ -6941,11 +6955,11 @@
   <sheetPr/>
   <dimension ref="A1:Y187"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="6" customWidth="1"/>
@@ -6996,7 +7010,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>854</v>
       </c>
@@ -7079,7 +7093,7 @@
     </row>
     <row r="5" s="3" customFormat="1" ht="44" customHeight="1" spans="1:25">
       <c r="A5" s="20" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>856</v>
@@ -7478,7 +7492,7 @@
     </row>
     <row r="16" s="3" customFormat="1" ht="32" customHeight="1" spans="1:25">
       <c r="A16" s="20" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>856</v>
@@ -7636,7 +7650,7 @@
         <v>49</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>794</v>
@@ -7663,7 +7677,7 @@
     </row>
     <row r="21" s="1" customFormat="1" ht="41" customHeight="1" spans="1:25">
       <c r="A21" s="20" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>856</v>
@@ -7678,7 +7692,7 @@
         <v>777</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="G21" s="27"/>
       <c r="H21" s="29"/>
@@ -7700,7 +7714,7 @@
       <c r="X21"/>
       <c r="Y21"/>
     </row>
-    <row r="22" s="4" customFormat="1" ht="27.6" spans="1:25">
+    <row r="22" s="4" customFormat="1" ht="28" spans="1:25">
       <c r="A22" s="20"/>
       <c r="B22" s="30" t="s">
         <v>858</v>
@@ -7801,7 +7815,7 @@
         <v>49</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F25" s="34" t="s">
         <v>794</v>
@@ -7861,7 +7875,7 @@
       <c r="N28" s="24"/>
       <c r="O28" s="23"/>
     </row>
-    <row r="29" customFormat="1" spans="8:15">
+    <row r="29" customFormat="1" ht="15.5" spans="8:15">
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="28"/>
@@ -7871,7 +7885,7 @@
       <c r="N29" s="24"/>
       <c r="O29" s="23"/>
     </row>
-    <row r="30" customFormat="1" spans="8:15">
+    <row r="30" customFormat="1" ht="15.5" spans="8:15">
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
       <c r="J30" s="28"/>
@@ -7881,7 +7895,7 @@
       <c r="N30" s="24"/>
       <c r="O30" s="23"/>
     </row>
-    <row r="31" customFormat="1" spans="8:15">
+    <row r="31" customFormat="1" ht="15.5" spans="8:15">
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
       <c r="J31" s="28"/>
@@ -7891,7 +7905,7 @@
       <c r="N31" s="24"/>
       <c r="O31" s="23"/>
     </row>
-    <row r="32" customFormat="1" spans="8:15">
+    <row r="32" customFormat="1" ht="15.5" spans="8:15">
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
       <c r="J32" s="28"/>
@@ -7943,7 +7957,7 @@
       <c r="N34" s="47"/>
       <c r="O34" s="46"/>
     </row>
-    <row r="35" customFormat="1" ht="15.6" spans="1:15">
+    <row r="35" customFormat="1" ht="15.5" spans="1:15">
       <c r="A35" s="20"/>
       <c r="B35" s="21"/>
       <c r="C35" s="26"/>
@@ -10821,7 +10835,7 @@
       <selection activeCell="C5" sqref="C5:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38" style="5" customWidth="1"/>
     <col min="2" max="2" width="44.125" style="6" customWidth="1"/>
@@ -10871,7 +10885,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>733</v>
       </c>
@@ -10952,7 +10966,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="5" s="55" customFormat="1" ht="32" customHeight="1" spans="1:16384">
+    <row r="5" s="56" customFormat="1" ht="32" customHeight="1" spans="1:16384">
       <c r="A5" s="20" t="s">
         <v>747</v>
       </c>
@@ -27400,7 +27414,7 @@
       <c r="N7" s="24"/>
       <c r="O7" s="23"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="28.8" spans="1:15">
+    <row r="8" s="1" customFormat="1" ht="29" spans="1:15">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
       <c r="C8" s="26" t="s">
@@ -27475,7 +27489,7 @@
       <c r="N10" s="24"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" s="4" customFormat="1" ht="15.6" spans="1:15">
+    <row r="11" s="4" customFormat="1" ht="15.5" spans="1:15">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="H11" s="29"/>
@@ -27487,7 +27501,7 @@
       <c r="N11" s="24"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" s="4" customFormat="1" ht="15.6" spans="1:15">
+    <row r="12" s="4" customFormat="1" ht="15.5" spans="1:15">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="H12" s="29"/>
@@ -27499,7 +27513,7 @@
       <c r="N12" s="24"/>
       <c r="O12" s="23"/>
     </row>
-    <row r="13" customFormat="1" ht="15.6" spans="1:15">
+    <row r="13" customFormat="1" ht="15.5" spans="1:15">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="H13" s="29"/>
@@ -27512,7 +27526,7 @@
       <c r="O13" s="23"/>
     </row>
     <row r="14" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A14" s="56"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="36"/>
       <c r="H14" s="35"/>
       <c r="I14" s="35"/>
@@ -27524,13 +27538,13 @@
       <c r="O14" s="46"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A15" s="56"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="36"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="59"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
       <c r="J15" s="45"/>
@@ -27541,9 +27555,9 @@
       <c r="O15" s="46"/>
     </row>
     <row r="16" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A16" s="56"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="36"/>
-      <c r="C16" s="60"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="35"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
@@ -27558,12 +27572,12 @@
       <c r="O16" s="46"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A17" s="56"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="63"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="35"/>
       <c r="H17" s="35"/>
       <c r="I17" s="35"/>
@@ -27695,7 +27709,7 @@
     </row>
     <row r="25" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="20"/>
-      <c r="B25" s="64"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="31"/>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
@@ -30692,11 +30706,11 @@
   <sheetPr/>
   <dimension ref="A1:Y185"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A11" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B19" sqref="B19:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="6" customWidth="1"/>
@@ -30747,7 +30761,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>759</v>
       </c>
@@ -31367,7 +31381,7 @@
       <c r="X22"/>
       <c r="Y22"/>
     </row>
-    <row r="23" s="4" customFormat="1" ht="15.6" spans="1:25">
+    <row r="23" s="4" customFormat="1" ht="15.5" spans="1:25">
       <c r="A23" s="20"/>
       <c r="B23" s="36"/>
       <c r="C23" s="31"/>
@@ -31523,7 +31537,7 @@
       <c r="N30" s="24"/>
       <c r="O30" s="23"/>
     </row>
-    <row r="31" customFormat="1" ht="15.6" spans="1:15">
+    <row r="31" customFormat="1" ht="15.5" spans="1:15">
       <c r="A31" s="20"/>
       <c r="B31" s="6"/>
       <c r="C31" s="26"/>
@@ -31574,7 +31588,7 @@
       <c r="N33" s="47"/>
       <c r="O33" s="46"/>
     </row>
-    <row r="34" customFormat="1" ht="15.6" spans="1:15">
+    <row r="34" customFormat="1" ht="15.5" spans="1:15">
       <c r="A34" s="20"/>
       <c r="B34" s="21"/>
       <c r="C34" s="26"/>
@@ -34461,11 +34475,11 @@
   <sheetPr/>
   <dimension ref="A1:O165"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="41.3333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="6" customWidth="1"/>
@@ -34516,7 +34530,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>798</v>
       </c>
@@ -34734,7 +34748,7 @@
       <c r="N9" s="24"/>
       <c r="O9" s="23"/>
     </row>
-    <row r="10" customFormat="1" ht="15.6" spans="1:15">
+    <row r="10" customFormat="1" ht="15.5" spans="1:15">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
         <v>806</v>
@@ -37854,10 +37868,10 @@
   <dimension ref="A1:Y182"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="6" customWidth="1"/>
@@ -37908,7 +37922,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>841</v>
       </c>
@@ -38348,7 +38362,7 @@
       <c r="X15"/>
       <c r="Y15"/>
     </row>
-    <row r="16" s="4" customFormat="1" ht="15.6" spans="1:25">
+    <row r="16" s="4" customFormat="1" ht="15.5" spans="1:25">
       <c r="A16" s="20"/>
       <c r="B16" s="36"/>
       <c r="C16" s="31"/>
@@ -38504,7 +38518,7 @@
       <c r="N23" s="24"/>
       <c r="O23" s="23"/>
     </row>
-    <row r="24" customFormat="1" ht="15.6" spans="1:15">
+    <row r="24" customFormat="1" ht="15.5" spans="1:15">
       <c r="A24" s="20"/>
       <c r="B24" s="6"/>
       <c r="C24" s="26"/>
@@ -38521,7 +38535,7 @@
       <c r="N24" s="24"/>
       <c r="O24" s="23"/>
     </row>
-    <row r="25" customFormat="1" ht="15.6" spans="1:15">
+    <row r="25" customFormat="1" ht="15.5" spans="1:15">
       <c r="A25" s="20"/>
       <c r="B25" s="6"/>
       <c r="C25" s="31"/>
@@ -38538,7 +38552,7 @@
       <c r="N25" s="24"/>
       <c r="O25" s="23"/>
     </row>
-    <row r="26" customFormat="1" ht="15.6" spans="1:15">
+    <row r="26" customFormat="1" ht="15.5" spans="1:15">
       <c r="A26" s="20"/>
       <c r="B26" s="6"/>
       <c r="C26" s="26"/>
@@ -38555,7 +38569,7 @@
       <c r="N26" s="24"/>
       <c r="O26" s="23"/>
     </row>
-    <row r="27" customFormat="1" ht="15.6" spans="1:15">
+    <row r="27" customFormat="1" ht="15.5" spans="1:15">
       <c r="A27" s="20"/>
       <c r="B27" s="6"/>
       <c r="C27" s="26"/>
@@ -38606,7 +38620,7 @@
       <c r="N29" s="47"/>
       <c r="O29" s="46"/>
     </row>
-    <row r="30" customFormat="1" ht="15.6" spans="1:15">
+    <row r="30" customFormat="1" ht="15.5" spans="1:15">
       <c r="A30" s="20"/>
       <c r="B30" s="21"/>
       <c r="C30" s="26"/>
@@ -41499,11 +41513,11 @@
   <sheetPr/>
   <dimension ref="A1:Y180"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G12"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="6" customWidth="1"/>
@@ -41554,7 +41568,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>854</v>
       </c>
@@ -41938,7 +41952,7 @@
       <c r="X13"/>
       <c r="Y13"/>
     </row>
-    <row r="14" s="4" customFormat="1" ht="15.6" spans="1:25">
+    <row r="14" s="4" customFormat="1" ht="15.5" spans="1:25">
       <c r="A14" s="20"/>
       <c r="B14" s="36"/>
       <c r="C14" s="31"/>
@@ -42094,7 +42108,7 @@
       <c r="N21" s="24"/>
       <c r="O21" s="23"/>
     </row>
-    <row r="22" customFormat="1" ht="15.6" spans="1:15">
+    <row r="22" customFormat="1" ht="15.5" spans="1:15">
       <c r="A22" s="20"/>
       <c r="B22" s="6"/>
       <c r="C22" s="26"/>
@@ -42111,7 +42125,7 @@
       <c r="N22" s="24"/>
       <c r="O22" s="23"/>
     </row>
-    <row r="23" customFormat="1" ht="15.6" spans="1:15">
+    <row r="23" customFormat="1" ht="15.5" spans="1:15">
       <c r="A23" s="20"/>
       <c r="B23" s="6"/>
       <c r="C23" s="31"/>
@@ -42128,7 +42142,7 @@
       <c r="N23" s="24"/>
       <c r="O23" s="23"/>
     </row>
-    <row r="24" customFormat="1" ht="15.6" spans="1:15">
+    <row r="24" customFormat="1" ht="15.5" spans="1:15">
       <c r="A24" s="20"/>
       <c r="B24" s="6"/>
       <c r="C24" s="26"/>
@@ -42145,7 +42159,7 @@
       <c r="N24" s="24"/>
       <c r="O24" s="23"/>
     </row>
-    <row r="25" customFormat="1" ht="15.6" spans="1:15">
+    <row r="25" customFormat="1" ht="15.5" spans="1:15">
       <c r="A25" s="20"/>
       <c r="B25" s="6"/>
       <c r="C25" s="26"/>
@@ -42196,7 +42210,7 @@
       <c r="N27" s="47"/>
       <c r="O27" s="46"/>
     </row>
-    <row r="28" customFormat="1" ht="15.6" spans="1:15">
+    <row r="28" customFormat="1" ht="15.5" spans="1:15">
       <c r="A28" s="20"/>
       <c r="B28" s="21"/>
       <c r="C28" s="26"/>
@@ -45089,11 +45103,11 @@
   <sheetPr/>
   <dimension ref="A1:Y185"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="6" customWidth="1"/>
@@ -45144,7 +45158,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>759</v>
       </c>
@@ -45673,9 +45687,11 @@
       <c r="Y18"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="23" customHeight="1" spans="1:25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="55" t="s">
+        <v>866</v>
+      </c>
       <c r="B19" s="21" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>5</v>
@@ -45712,7 +45728,7 @@
     <row r="20" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>5</v>
@@ -45724,7 +45740,7 @@
         <v>768</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="G20" s="29"/>
       <c r="H20" s="35"/>
@@ -45748,10 +45764,10 @@
         <v>471</v>
       </c>
       <c r="E21" s="50" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
@@ -45773,7 +45789,7 @@
       <c r="X21"/>
       <c r="Y21"/>
     </row>
-    <row r="22" s="4" customFormat="1" ht="15.6" spans="1:25">
+    <row r="22" s="4" customFormat="1" ht="28" spans="1:25">
       <c r="A22" s="20"/>
       <c r="B22" s="21" t="s">
         <v>773</v>
@@ -45820,10 +45836,10 @@
         <v>471</v>
       </c>
       <c r="E23" s="50" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G23" s="29"/>
       <c r="H23" s="35"/>
@@ -45886,7 +45902,7 @@
         <v>780</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
@@ -45999,7 +46015,7 @@
         <v>49</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F29" s="34" t="s">
         <v>794</v>
@@ -46039,7 +46055,7 @@
       <c r="N30" s="24"/>
       <c r="O30" s="23"/>
     </row>
-    <row r="31" customFormat="1" ht="15.6" spans="1:15">
+    <row r="31" customFormat="1" ht="15.5" spans="1:15">
       <c r="A31" s="20"/>
       <c r="B31" s="30" t="s">
         <v>796</v>
@@ -46098,7 +46114,7 @@
       <c r="N33" s="47"/>
       <c r="O33" s="46"/>
     </row>
-    <row r="34" customFormat="1" ht="15.6" spans="1:15">
+    <row r="34" customFormat="1" ht="15.5" spans="1:15">
       <c r="A34" s="20"/>
       <c r="B34" s="21"/>
       <c r="C34" s="26"/>
@@ -48986,11 +49002,11 @@
   <sheetPr/>
   <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:E55"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="41.3333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.375" style="6" customWidth="1"/>
@@ -49041,7 +49057,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>798</v>
       </c>
@@ -49124,7 +49140,7 @@
     </row>
     <row r="5" s="53" customFormat="1" ht="40" customHeight="1" spans="1:15">
       <c r="A5" s="20" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>800</v>
@@ -49161,7 +49177,7 @@
         <v>465</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>767</v>
@@ -49230,7 +49246,7 @@
       <c r="N8" s="24"/>
       <c r="O8" s="23"/>
     </row>
-    <row r="9" customFormat="1" ht="15.6" spans="1:15">
+    <row r="9" customFormat="1" ht="15.5" spans="1:15">
       <c r="A9" s="20"/>
       <c r="B9" s="21" t="s">
         <v>806</v>
@@ -49392,7 +49408,7 @@
     </row>
     <row r="15" s="1" customFormat="1" ht="52" customHeight="1" spans="1:15">
       <c r="A15" s="20" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>828</v>
@@ -49407,7 +49423,7 @@
         <v>777</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -49527,7 +49543,7 @@
     </row>
     <row r="20" s="1" customFormat="1" ht="42" customHeight="1" spans="1:15">
       <c r="A20" s="20" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>833</v>
@@ -49542,7 +49558,7 @@
         <v>777</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="G20" s="29"/>
       <c r="H20" s="29"/>
@@ -49662,7 +49678,7 @@
     </row>
     <row r="25" s="1" customFormat="1" ht="43" customHeight="1" spans="1:15">
       <c r="A25" s="20" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>833</v>
@@ -49677,7 +49693,7 @@
         <v>777</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="29"/>
@@ -49826,7 +49842,7 @@
     </row>
     <row r="31" s="1" customFormat="1" ht="39" customHeight="1" spans="1:15">
       <c r="A31" s="20" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>800</v>
@@ -49863,7 +49879,7 @@
         <v>465</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>767</v>
@@ -49920,7 +49936,7 @@
         <v>777</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="G34" s="29"/>
       <c r="H34" s="29"/>
@@ -50023,7 +50039,7 @@
         <v>49</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F38" s="34" t="s">
         <v>794</v>
@@ -50067,7 +50083,7 @@
     </row>
     <row r="40" s="1" customFormat="1" ht="52" customHeight="1" spans="1:15">
       <c r="A40" s="20" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>828</v>
@@ -50082,7 +50098,7 @@
         <v>777</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="G40" s="29"/>
       <c r="H40" s="29"/>
@@ -50185,7 +50201,7 @@
         <v>49</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F44" s="34" t="s">
         <v>794</v>
@@ -50202,7 +50218,7 @@
     </row>
     <row r="45" s="1" customFormat="1" ht="48" customHeight="1" spans="1:15">
       <c r="A45" s="20" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>833</v>
@@ -50217,7 +50233,7 @@
         <v>777</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="G45" s="29"/>
       <c r="H45" s="29"/>
@@ -50337,7 +50353,7 @@
     </row>
     <row r="50" s="1" customFormat="1" ht="44" customHeight="1" spans="1:15">
       <c r="A50" s="20" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B50" s="21" t="s">
         <v>833</v>
@@ -50352,7 +50368,7 @@
         <v>777</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="29"/>
@@ -50455,7 +50471,7 @@
         <v>49</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F54" s="34" t="s">
         <v>794</v>
@@ -52228,11 +52244,11 @@
   <sheetPr/>
   <dimension ref="A1:Y194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="48.9333333333333" style="6" customWidth="1"/>
@@ -52283,7 +52299,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="39"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
         <v>841</v>
       </c>
@@ -52366,7 +52382,7 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="47" customHeight="1" spans="1:15">
       <c r="A5" s="20" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>842</v>
@@ -52635,7 +52651,7 @@
     </row>
     <row r="13" s="49" customFormat="1" ht="42" customHeight="1" spans="1:15">
       <c r="A13" s="20" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>763</v>
@@ -52672,10 +52688,10 @@
         <v>471</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="G14" s="29"/>
       <c r="H14" s="35"/>
@@ -52697,7 +52713,7 @@
         <v>536</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="29"/>
@@ -52713,7 +52729,7 @@
     <row r="16" s="49" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="20"/>
       <c r="B16" s="21" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>5</v>
@@ -52722,7 +52738,7 @@
         <v>465</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F16" s="34" t="s">
         <v>767</v>
@@ -52740,7 +52756,7 @@
     <row r="17" s="49" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="20"/>
       <c r="B17" s="21" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>5</v>
@@ -52752,7 +52768,7 @@
         <v>768</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="G17" s="29"/>
       <c r="H17" s="35"/>
@@ -52767,7 +52783,7 @@
     <row r="18" s="49" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="20"/>
       <c r="B18" s="21" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>5</v>
@@ -52776,10 +52792,10 @@
         <v>471</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="G18" s="29"/>
       <c r="H18" s="35"/>
@@ -52824,7 +52840,7 @@
         <v>536</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="29"/>
@@ -52840,7 +52856,7 @@
     <row r="21" s="49" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>5</v>
@@ -52849,10 +52865,10 @@
         <v>471</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="G21" s="29"/>
       <c r="H21" s="35"/>
@@ -52874,7 +52890,7 @@
         <v>536</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="29"/>
@@ -52890,7 +52906,7 @@
     <row r="23" s="49" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="20"/>
       <c r="B23" s="21" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>5</v>
@@ -52899,10 +52915,10 @@
         <v>471</v>
       </c>
       <c r="E23" s="50" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G23" s="29"/>
       <c r="H23" s="35"/>
@@ -52924,7 +52940,7 @@
         <v>536</v>
       </c>
       <c r="E24" s="50" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="29"/>
@@ -52940,7 +52956,7 @@
     <row r="25" s="49" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="52"/>
       <c r="B25" s="21" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>5</v>
@@ -52949,10 +52965,10 @@
         <v>471</v>
       </c>
       <c r="E25" s="50" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="35"/>
@@ -52974,7 +52990,7 @@
         <v>536</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="29"/>
@@ -53001,7 +53017,7 @@
         <v>780</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="G27" s="29"/>
       <c r="H27" s="35"/>
@@ -53038,7 +53054,7 @@
         <v>777</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
@@ -53142,7 +53158,7 @@
         <v>49</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>794</v>
@@ -53170,7 +53186,7 @@
     <row r="33" s="1" customFormat="1" ht="23" customHeight="1" spans="1:25">
       <c r="A33" s="20"/>
       <c r="B33" s="21" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>20</v>
@@ -53246,7 +53262,7 @@
       <c r="N35" s="24"/>
       <c r="O35" s="23"/>
     </row>
-    <row r="36" customFormat="1" ht="15.6" spans="1:15">
+    <row r="36" customFormat="1" ht="15.5" spans="1:15">
       <c r="A36" s="20"/>
       <c r="B36" s="6"/>
       <c r="C36" s="26"/>
@@ -53263,7 +53279,7 @@
       <c r="N36" s="24"/>
       <c r="O36" s="23"/>
     </row>
-    <row r="37" customFormat="1" ht="15.6" spans="1:15">
+    <row r="37" customFormat="1" ht="15.5" spans="1:15">
       <c r="A37" s="20"/>
       <c r="B37" s="6"/>
       <c r="C37" s="31"/>
@@ -53280,7 +53296,7 @@
       <c r="N37" s="24"/>
       <c r="O37" s="23"/>
     </row>
-    <row r="38" customFormat="1" ht="15.6" spans="1:15">
+    <row r="38" customFormat="1" ht="15.5" spans="1:15">
       <c r="A38" s="20"/>
       <c r="B38" s="6"/>
       <c r="C38" s="26"/>
@@ -53297,7 +53313,7 @@
       <c r="N38" s="24"/>
       <c r="O38" s="23"/>
     </row>
-    <row r="39" customFormat="1" ht="15.6" spans="1:15">
+    <row r="39" customFormat="1" ht="15.5" spans="1:15">
       <c r="A39" s="20"/>
       <c r="B39" s="6"/>
       <c r="C39" s="26"/>
@@ -53348,7 +53364,7 @@
       <c r="N41" s="47"/>
       <c r="O41" s="46"/>
     </row>
-    <row r="42" customFormat="1" ht="15.6" spans="1:15">
+    <row r="42" customFormat="1" ht="15.5" spans="1:15">
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="26"/>

</xml_diff>